<commit_message>
Added updateCard and hooked it up to GUI
</commit_message>
<xml_diff>
--- a/out/production/AnkiChess/TestData.xlsx
+++ b/out/production/AnkiChess/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jackv\IdeaProjects\AnkiChess\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{209EFFA7-E872-4C5C-BD5D-F80C9DA83F88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{107E0F53-D673-4D45-8961-031FD8F3C087}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-90" windowWidth="14400" windowHeight="7350" firstSheet="2" activeTab="2" xr2:uid="{D49D661D-D964-4DF3-8EF7-F73922AC7FB4}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="7350" activeTab="1" xr2:uid="{D49D661D-D964-4DF3-8EF7-F73922AC7FB4}"/>
   </bookViews>
   <sheets>
     <sheet name="DECKS" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="43">
   <si>
     <t>ID</t>
   </si>
@@ -163,6 +163,12 @@
   </si>
   <si>
     <t>BOTEZ GAMBIT</t>
+  </si>
+  <si>
+    <t>LAST_REVIEW</t>
+  </si>
+  <si>
+    <t>MILLIS</t>
   </si>
 </sst>
 </file>
@@ -562,15 +568,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD9DBC98-5124-4672-BE1C-28C519D504C5}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="19.36328125" customWidth="1"/>
+    <col min="4" max="4" width="17.453125" customWidth="1"/>
+    <col min="5" max="5" width="15.54296875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -586,8 +597,11 @@
       <c r="E1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -603,8 +617,11 @@
       <c r="E2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -620,8 +637,11 @@
       <c r="E3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -637,8 +657,11 @@
       <c r="E4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -654,8 +677,11 @@
       <c r="E5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -671,8 +697,11 @@
       <c r="E6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -688,8 +717,11 @@
       <c r="E7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -705,8 +737,11 @@
       <c r="E8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -722,8 +757,11 @@
       <c r="E9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -739,8 +777,11 @@
       <c r="E10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -755,6 +796,9 @@
       </c>
       <c r="E11">
         <v>0</v>
+      </c>
+      <c r="F11" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -766,7 +810,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{472ACACB-E0B8-437B-B106-D85EA7F88376}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>

</xml_diff>